<commit_message>
the upstream and downstream process objects are added to the objects and the code is refactored for better structuring
objects mapped to upstream and downstream
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Order.xlsx
+++ b/customSim/LES/systemDefinition/Order.xlsx
@@ -15,9 +15,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -34,9 +35,8 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
-      <scheme val="minor"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -83,17 +83,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,34 +471,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>env</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>order_date</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>order_id</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>product</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -503,7 +506,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>45317</v>
       </c>
       <c r="D2" t="inlineStr">
@@ -523,7 +526,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -531,7 +534,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="6" t="n">
         <v>45320</v>
       </c>
       <c r="D3" t="inlineStr">
@@ -551,7 +554,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -559,7 +562,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <v>45328</v>
       </c>
       <c r="D4" t="inlineStr">
@@ -579,7 +582,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -587,7 +590,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>45332</v>
       </c>
       <c r="D5" t="inlineStr">
@@ -607,7 +610,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -615,7 +618,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>45341</v>
       </c>
       <c r="D6" t="inlineStr">
@@ -635,7 +638,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -643,7 +646,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>45350</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -663,7 +666,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -671,7 +674,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>45357</v>
       </c>
       <c r="D8" t="inlineStr">
@@ -691,7 +694,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -699,7 +702,7 @@
           <t>env</t>
         </is>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <v>45359</v>
       </c>
       <c r="D9" t="inlineStr">

</xml_diff>